<commit_message>
adding csv team players parser, need fixing
</commit_message>
<xml_diff>
--- a/TeamsData.xlsx
+++ b/TeamsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaka/V_League/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF681B-AA21-8D4A-BEB5-FD821C0F7C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1867AFCB-126C-B948-BE65-88798BB57D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{F8FB08C7-AA83-8542-974F-76205D103565}"/>
+    <workbookView xWindow="37280" yWindow="-800" windowWidth="28040" windowHeight="16940" xr2:uid="{F8FB08C7-AA83-8542-974F-76205D103565}"/>
   </bookViews>
   <sheets>
     <sheet name="Hong Linh Ha Tinh" sheetId="1" r:id="rId1"/>
@@ -554,15 +554,14 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.25">
@@ -570,19 +569,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -592,20 +591,20 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
       </c>
       <c r="G2">
         <v>28</v>
@@ -615,20 +614,20 @@
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
       </c>
       <c r="G3">
         <v>23</v>
@@ -638,20 +637,20 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
       </c>
       <c r="G4">
         <v>29</v>
@@ -661,40 +660,40 @@
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="2">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G6">
         <v>29</v>
@@ -704,20 +703,20 @@
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="2">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G7">
         <v>34</v>
@@ -727,20 +726,20 @@
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="2">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G8">
         <v>26</v>
@@ -750,20 +749,20 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2">
         <v>9</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
       </c>
       <c r="G9">
         <v>26</v>
@@ -773,20 +772,20 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="2">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
-        <v>16</v>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
+      <c r="F10" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G10">
         <v>30</v>
@@ -796,20 +795,20 @@
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
+      <c r="B11" s="2">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G11">
         <v>28</v>
@@ -819,20 +818,20 @@
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="2">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
-        <v>16</v>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G12">
         <v>30</v>
@@ -842,20 +841,20 @@
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C13" s="2">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
       </c>
       <c r="G13">
         <v>29</v>
@@ -865,20 +864,20 @@
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
+      <c r="B14" s="2">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>0</v>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G14">
         <v>25</v>
@@ -888,20 +887,20 @@
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C15" s="2">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
       </c>
       <c r="G15">
         <v>26</v>
@@ -911,20 +910,20 @@
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C16" s="2">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
       </c>
       <c r="G16">
         <v>28</v>
@@ -934,20 +933,20 @@
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="2">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
-        <v>16</v>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>0</v>
+      <c r="F17" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G17">
         <v>26</v>
@@ -957,20 +956,20 @@
       <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" s="2">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
       </c>
       <c r="G18">
         <v>31</v>
@@ -980,20 +979,20 @@
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="2">
         <v>21</v>
       </c>
-      <c r="D19" t="s">
-        <v>16</v>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
-        <v>0</v>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G19">
         <v>24</v>
@@ -1003,60 +1002,60 @@
       <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C20" s="2">
-        <v>23</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C21" s="2">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C22" s="2">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
       </c>
       <c r="G22">
         <v>26</v>
@@ -1066,20 +1065,20 @@
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="2">
         <v>27</v>
       </c>
-      <c r="D23" t="s">
-        <v>16</v>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>0</v>
+      <c r="F23" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G23">
         <v>30</v>
@@ -1089,20 +1088,20 @@
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C24" s="2">
-        <v>28</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
       </c>
       <c r="G24">
         <v>29</v>
@@ -1112,40 +1111,40 @@
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="2">
         <v>29</v>
       </c>
-      <c r="D25" t="s">
-        <v>16</v>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>0</v>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="2">
         <v>37</v>
       </c>
-      <c r="D26" t="s">
-        <v>16</v>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
-        <v>0</v>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G26">
         <v>23</v>
@@ -1155,20 +1154,20 @@
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C27" s="2">
-        <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
       </c>
       <c r="G27">
         <v>19</v>
@@ -1178,20 +1177,20 @@
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="2">
         <v>77</v>
       </c>
-      <c r="D28" t="s">
-        <v>16</v>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="F28" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G28">
         <v>25</v>
@@ -1201,20 +1200,20 @@
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="2">
         <v>88</v>
       </c>
-      <c r="D29" t="s">
-        <v>16</v>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G29">
         <v>24</v>
@@ -1224,20 +1223,20 @@
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C30" s="2">
-        <v>92</v>
-      </c>
-      <c r="D30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
       </c>
       <c r="G30">
         <v>29</v>
@@ -1247,20 +1246,20 @@
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C31" s="2">
-        <v>97</v>
-      </c>
-      <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
       </c>
       <c r="G31">
         <v>24</v>

</xml_diff>